<commit_message>
Docs: - changed clothes sizes - no tm added to categories - crm maanger and agent external problem badge
</commit_message>
<xml_diff>
--- a/app/download_dir/одежда_по каждому размеру.xlsx
+++ b/app/download_dir/одежда_по каждому размеру.xlsx
@@ -1222,7 +1222,7 @@
     <t xml:space="preserve">ТЕРРАКОТОВЫЙ</t>
   </si>
   <si>
-    <t xml:space="preserve">ОДИН РАЗМЕР</t>
+    <t xml:space="preserve">ЕДИНЫЙ РАЗМЕР</t>
   </si>
   <si>
     <t xml:space="preserve">ИРАН (ИСЛАМСКАЯ РЕСПУБЛИКА)</t>
@@ -6228,7 +6228,7 @@
       <selection pane="topLeft" activeCell="R1600" activeCellId="0" sqref="R1600"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.33"/>
@@ -18880,11 +18880,11 @@
   </sheetPr>
   <dimension ref="A1:J246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D104" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H108" activeCellId="0" sqref="H108"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D74" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H85" activeCellId="0" sqref="H85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -22210,7 +22210,7 @@
       <selection pane="topLeft" activeCell="A751" activeCellId="0" sqref="A751"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="240.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="241.1484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>

</xml_diff>